<commit_message>
Update data: add rebounds & 3-pointers
</commit_message>
<xml_diff>
--- a/Atlanta_Hawks_2025-26_stats.xlsx
+++ b/Atlanta_Hawks_2025-26_stats.xlsx
@@ -9,8 +9,12 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Points" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assists" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg Points" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg Assists" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Rebounds" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="3PM" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg Points" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg Assists" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg Rebounds" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg 3PM" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1894,7 +1898,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1905,163 +1909,715 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Player</t>
+          <t>Game Time (PST)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Avg Points</t>
+          <t>Opponent</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jacob Toppin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Jalen Johnson</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Keaton Wallace</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luke Kennard</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Dyson Daniels</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Kristaps Porziņģis</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Zaccharie Risacher</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Trae Young</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>N'Faly Dante</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Asa Newell</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Onyeka Okongwu</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Mouhamed Gueye</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Vít Krejčí</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Caleb Houstan</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Jalen Johnson</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>20.11111111111111</v>
+          <t>2025-10-22</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I2" t="n">
+        <v>7</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>6</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kristaps Porziņģis</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>17.875</v>
+          <t>2025-10-24</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>4</v>
+      </c>
+      <c r="O3" t="n">
+        <v>8</v>
+      </c>
+      <c r="P3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Trae Young</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>17.8</v>
+          <t>2025-10-25</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OKC</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>4</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="n">
+        <v>4</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N4" t="n">
+        <v>12</v>
+      </c>
+      <c r="O4" t="n">
+        <v>6</v>
+      </c>
+      <c r="P4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nickeil Alexander-Walker</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>17.55555555555556</v>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CHI</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7</v>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>3</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>10</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Onyeka Okongwu</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>12.72727272727273</v>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>7</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" t="n">
+        <v>6</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>14</v>
+      </c>
+      <c r="O6" t="n">
+        <v>4</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Zaccharie Risacher</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>12.66666666666667</v>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>13</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>9</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>8</v>
+      </c>
+      <c r="J7" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>9</v>
+      </c>
+      <c r="O7" t="n">
+        <v>6</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Vít Krejčí</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>10.42857142857143</v>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>13</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" t="n">
+        <v>12</v>
+      </c>
+      <c r="J8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>5</v>
+      </c>
+      <c r="O8" t="n">
+        <v>3</v>
+      </c>
+      <c r="P8" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dyson Daniels</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>9.454545454545455</v>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
+        <v>6</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="n">
+        <v>4</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>7</v>
+      </c>
+      <c r="O9" t="n">
+        <v>3</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Luke Kennard</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>8.333333333333334</v>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>7</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="n">
+        <v>7</v>
+      </c>
+      <c r="J10" t="n">
+        <v>5</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>11</v>
+      </c>
+      <c r="O10" t="n">
+        <v>7</v>
+      </c>
+      <c r="P10" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mouhamed Gueye</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
+          <t>2025-11-08</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>LAL</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>5</v>
+      </c>
+      <c r="N11" t="n">
+        <v>8</v>
+      </c>
+      <c r="O11" t="n">
         <v>7</v>
+      </c>
+      <c r="P11" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Asa Newell</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Keaton Wallace</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Jacob Toppin</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Caleb Houstan</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>N'Faly Dante</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.75</v>
+          <t>2025-11-10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>3</v>
+      </c>
+      <c r="J12" t="n">
+        <v>5</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>6</v>
+      </c>
+      <c r="O12" t="n">
+        <v>3</v>
+      </c>
+      <c r="P12" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2070,6 +2626,739 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Game Time (PST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Opponent</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jacob Toppin</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Jalen Johnson</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Keaton Wallace</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Luke Kennard</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Dyson Daniels</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Kristaps Porziņģis</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Zaccharie Risacher</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Trae Young</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>N'Faly Dante</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Asa Newell</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Onyeka Okongwu</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Mouhamed Gueye</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Vít Krejčí</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Caleb Houstan</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-10-22</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-10-24</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-10-25</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OKC</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
+      </c>
+      <c r="N4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O4" t="n">
+        <v>2</v>
+      </c>
+      <c r="P4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CHI</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>2</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>2</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>1</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>3</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>2</v>
+      </c>
+      <c r="O9" t="n">
+        <v>1</v>
+      </c>
+      <c r="P9" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-11-08</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>LAL</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>3</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>2</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>4</v>
+      </c>
+      <c r="P11" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-11-10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2091,13 +3380,194 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Avg Assists</t>
+          <t>Avg Points</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Jalen Johnson</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>20.11111111111111</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kristaps Porziņģis</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>17.875</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Trae Young</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>17.55555555555556</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Onyeka Okongwu</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>12.72727272727273</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Zaccharie Risacher</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>12.66666666666667</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Vít Krejčí</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>10.42857142857143</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Dyson Daniels</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>9.454545454545455</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Luke Kennard</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>8.333333333333334</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mouhamed Gueye</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Asa Newell</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Keaton Wallace</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Jacob Toppin</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Caleb Houstan</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>N'Faly Dante</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Avg Assists</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>Trae Young</t>
         </is>
       </c>
@@ -2223,6 +3693,368 @@
       </c>
       <c r="B14" t="n">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Jacob Toppin</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>N'Faly Dante</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Avg Rebounds</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Jalen Johnson</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>8.555555555555555</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Onyeka Okongwu</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>8.363636363636363</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Dyson Daniels</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>5.909090909090909</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kristaps Porziņģis</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5.875</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Mouhamed Gueye</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4.272727272727272</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Asa Newell</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>2.555555555555555</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Zaccharie Risacher</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2.555555555555555</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Vít Krejčí</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2.428571428571428</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Luke Kennard</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>2.333333333333333</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Keaton Wallace</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Trae Young</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>N'Faly Dante</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Caleb Houstan</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Jacob Toppin</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Player</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Avg 3PM</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Vít Krejčí</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2.285714285714286</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Nickeil Alexander-Walker</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Zaccharie Risacher</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1.666666666666667</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kristaps Porziņģis</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Luke Kennard</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1.222222222222222</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Keaton Wallace</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Asa Newell</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Trae Young</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Onyeka Okongwu</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Mouhamed Gueye</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9090909090909091</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Jalen Johnson</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.5555555555555556</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Dyson Daniels</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.2727272727272727</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Caleb Houstan</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="15">

</xml_diff>

<commit_message>
Add openpyxl, pin Python 3.11, set Excel engine
</commit_message>
<xml_diff>
--- a/Atlanta_Hawks_2025-26_stats.xlsx
+++ b/Atlanta_Hawks_2025-26_stats.xlsx
@@ -15,6 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg Assists" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg Rebounds" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg 3PM" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Team Points" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1151,6 +1152,120 @@
         <v>28</v>
       </c>
       <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SAC</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>24</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>13</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5</v>
+      </c>
+      <c r="H13" t="n">
+        <v>14</v>
+      </c>
+      <c r="I13" t="n">
+        <v>13</v>
+      </c>
+      <c r="J13" t="n">
+        <v>15</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>5</v>
+      </c>
+      <c r="N13" t="n">
+        <v>21</v>
+      </c>
+      <c r="O13" t="n">
+        <v>2</v>
+      </c>
+      <c r="P13" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>UTA</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>31</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>16</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>11</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>32</v>
+      </c>
+      <c r="O14" t="n">
+        <v>8</v>
+      </c>
+      <c r="P14" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1165,7 +1280,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1884,6 +1999,120 @@
         <v>2</v>
       </c>
       <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SAC</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>8</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8</v>
+      </c>
+      <c r="H13" t="n">
+        <v>4</v>
+      </c>
+      <c r="I13" t="n">
+        <v>6</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2</v>
+      </c>
+      <c r="O13" t="n">
+        <v>2</v>
+      </c>
+      <c r="P13" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>UTA</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>14</v>
+      </c>
+      <c r="E14" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>2</v>
+      </c>
+      <c r="O14" t="n">
+        <v>1</v>
+      </c>
+      <c r="P14" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1898,7 +2127,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2617,6 +2846,120 @@
         <v>3</v>
       </c>
       <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SAC</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>6</v>
+      </c>
+      <c r="H13" t="n">
+        <v>6</v>
+      </c>
+      <c r="I13" t="n">
+        <v>4</v>
+      </c>
+      <c r="J13" t="n">
+        <v>3</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" t="n">
+        <v>3</v>
+      </c>
+      <c r="P13" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>UTA</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>18</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>3</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>11</v>
+      </c>
+      <c r="O14" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2631,7 +2974,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3350,6 +3693,120 @@
         <v>8</v>
       </c>
       <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SAC</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>1</v>
+      </c>
+      <c r="N13" t="n">
+        <v>2</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>UTA</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>4</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>8</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3391,27 +3848,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20.11111111111111</v>
+        <v>21.45454545454545</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kristaps Porziņģis</t>
+          <t>Trae Young</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>17.875</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Trae Young</t>
+          <t>Kristaps Porziņģis</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>17.8</v>
+        <v>17.33333333333333</v>
       </c>
     </row>
     <row r="5">
@@ -3421,7 +3878,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.55555555555556</v>
+        <v>17.09090909090909</v>
       </c>
     </row>
     <row r="6">
@@ -3431,7 +3888,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12.72727272727273</v>
+        <v>14.84615384615385</v>
       </c>
     </row>
     <row r="7">
@@ -3441,7 +3898,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>12.66666666666667</v>
+        <v>12.72727272727273</v>
       </c>
     </row>
     <row r="8">
@@ -3451,27 +3908,27 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10.42857142857143</v>
+        <v>11.55555555555556</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Dyson Daniels</t>
+          <t>Luke Kennard</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>9.454545454545455</v>
+        <v>9.090909090909092</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Luke Kennard</t>
+          <t>Dyson Daniels</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8.333333333333334</v>
+        <v>8.538461538461538</v>
       </c>
     </row>
     <row r="11">
@@ -3481,7 +3938,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>6.692307692307693</v>
       </c>
     </row>
     <row r="12">
@@ -3491,7 +3948,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6.8</v>
+        <v>5.571428571428571</v>
       </c>
     </row>
     <row r="13">
@@ -3501,23 +3958,23 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5.2</v>
+        <v>4.666666666666667</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Jacob Toppin</t>
+          <t>Caleb Houstan</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Caleb Houstan</t>
+          <t>Jacob Toppin</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -3578,21 +4035,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dyson Daniels</t>
+          <t>Jalen Johnson</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5.363636363636363</v>
+        <v>6.272727272727272</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Jalen Johnson</t>
+          <t>Dyson Daniels</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.222222222222222</v>
+        <v>5.384615384615385</v>
       </c>
     </row>
     <row r="5">
@@ -3602,7 +4059,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.375</v>
+        <v>3.666666666666667</v>
       </c>
     </row>
     <row r="6">
@@ -3612,7 +4069,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.222222222222222</v>
+        <v>3.454545454545455</v>
       </c>
     </row>
     <row r="7">
@@ -3622,7 +4079,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.9</v>
+        <v>3.166666666666667</v>
       </c>
     </row>
     <row r="8">
@@ -3632,7 +4089,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.363636363636364</v>
+        <v>2.307692307692307</v>
       </c>
     </row>
     <row r="9">
@@ -3642,27 +4099,27 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>1.909090909090909</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mouhamed Gueye</t>
+          <t>Vít Krejčí</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1.545454545454545</v>
+        <v>1.777777777777778</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Vít Krejčí</t>
+          <t>Mouhamed Gueye</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1.285714285714286</v>
+        <v>1.538461538461539</v>
       </c>
     </row>
     <row r="12">
@@ -3672,7 +4129,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1.222222222222222</v>
+        <v>1.272727272727273</v>
       </c>
     </row>
     <row r="13">
@@ -3682,7 +4139,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14">
@@ -3692,7 +4149,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.2</v>
+        <v>0.1428571428571428</v>
       </c>
     </row>
     <row r="15">
@@ -3753,7 +4210,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8.555555555555555</v>
+        <v>9.545454545454545</v>
       </c>
     </row>
     <row r="3">
@@ -3763,27 +4220,27 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8.363636363636363</v>
+        <v>8.153846153846153</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Dyson Daniels</t>
+          <t>Kristaps Porziņģis</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5.909090909090909</v>
+        <v>5.666666666666667</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kristaps Porziņģis</t>
+          <t>Dyson Daniels</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5.875</v>
+        <v>5.615384615384615</v>
       </c>
     </row>
     <row r="6">
@@ -3793,37 +4250,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.272727272727272</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Asa Newell</t>
+          <t>Nickeil Alexander-Walker</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>2.818181818181818</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Nickeil Alexander-Walker</t>
+          <t>Zaccharie Risacher</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.555555555555555</v>
+        <v>2.636363636363636</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Zaccharie Risacher</t>
+          <t>Luke Kennard</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2.555555555555555</v>
+        <v>2.363636363636364</v>
       </c>
     </row>
     <row r="10">
@@ -3833,17 +4290,17 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2.428571428571428</v>
+        <v>2.333333333333333</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Luke Kennard</t>
+          <t>Asa Newell</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.333333333333333</v>
+        <v>2.285714285714286</v>
       </c>
     </row>
     <row r="12">
@@ -3883,7 +4340,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="16">
@@ -3934,7 +4391,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.285714285714286</v>
+        <v>2.777777777777778</v>
       </c>
     </row>
     <row r="3">
@@ -3944,63 +4401,63 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>1.818181818181818</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Zaccharie Risacher</t>
+          <t>Luke Kennard</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.666666666666667</v>
+        <v>1.636363636363636</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kristaps Porziņģis</t>
+          <t>Onyeka Okongwu</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1.5</v>
+        <v>1.615384615384615</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Luke Kennard</t>
+          <t>Kristaps Porziņģis</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1.222222222222222</v>
+        <v>1.555555555555556</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Keaton Wallace</t>
+          <t>Zaccharie Risacher</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.2</v>
+        <v>1.545454545454545</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Asa Newell</t>
+          <t>Jalen Johnson</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Trae Young</t>
+          <t>Keaton Wallace</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -4010,7 +4467,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Onyeka Okongwu</t>
+          <t>Trae Young</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -4020,41 +4477,41 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mouhamed Gueye</t>
+          <t>Asa Newell</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9090909090909091</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Jalen Johnson</t>
+          <t>Mouhamed Gueye</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.5555555555555556</v>
+        <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Dyson Daniels</t>
+          <t>Caleb Houstan</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Caleb Houstan</t>
+          <t>Dyson Daniels</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.25</v>
+        <v>0.2307692307692308</v>
       </c>
     </row>
     <row r="15">
@@ -4075,6 +4532,325 @@
       </c>
       <c r="B16" t="n">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Game Time (PST)</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Opponent</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Team Points</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Opponent Points</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Game Total Points</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-10-22</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>118</v>
+      </c>
+      <c r="D2" t="n">
+        <v>138</v>
+      </c>
+      <c r="E2" t="n">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-10-24</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>111</v>
+      </c>
+      <c r="D3" t="n">
+        <v>107</v>
+      </c>
+      <c r="E3" t="n">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-10-25</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OKC</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>100</v>
+      </c>
+      <c r="D4" t="n">
+        <v>117</v>
+      </c>
+      <c r="E4" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-10-27</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>CHI</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>123</v>
+      </c>
+      <c r="D5" t="n">
+        <v>128</v>
+      </c>
+      <c r="E5" t="n">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-10-29</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>117</v>
+      </c>
+      <c r="D6" t="n">
+        <v>112</v>
+      </c>
+      <c r="E6" t="n">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-10-31</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>IND</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>128</v>
+      </c>
+      <c r="D7" t="n">
+        <v>108</v>
+      </c>
+      <c r="E7" t="n">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>109</v>
+      </c>
+      <c r="D8" t="n">
+        <v>117</v>
+      </c>
+      <c r="E8" t="n">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-11-04</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ORL</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>127</v>
+      </c>
+      <c r="D9" t="n">
+        <v>112</v>
+      </c>
+      <c r="E9" t="n">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>97</v>
+      </c>
+      <c r="D10" t="n">
+        <v>109</v>
+      </c>
+      <c r="E10" t="n">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-11-08</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>LAL</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>122</v>
+      </c>
+      <c r="D11" t="n">
+        <v>102</v>
+      </c>
+      <c r="E11" t="n">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-11-10</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>105</v>
+      </c>
+      <c r="D12" t="n">
+        <v>102</v>
+      </c>
+      <c r="E12" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-11-12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>SAC</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>133</v>
+      </c>
+      <c r="D13" t="n">
+        <v>100</v>
+      </c>
+      <c r="E13" t="n">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-11-13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>UTA</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>132</v>
+      </c>
+      <c r="D14" t="n">
+        <v>122</v>
+      </c>
+      <c r="E14" t="n">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>